<commit_message>
output_processor updated to include engine, crsr connections to database. full table uploaded to database
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,147 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dokiu\OneDrive\Documents\DSCubed\ai-at-dscubed\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045F0E28-84B0-4B83-BA7E-CD65EA91B957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>topic_name</t>
-  </si>
-  <si>
-    <t>topic_description</t>
-  </si>
-  <si>
-    <t>Meeting Info</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Meeting Summary**
-**Date:** [Not specified]  
-**Participants:** Aaron, Andy L, Andy S, Arnav, Chi, Fairy, Karen
-</t>
-  </si>
-  <si>
-    <t>### 1. Main Topics Discussed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- **AI@DSCubed Website Redesign**
-- **Discord Bot Enhancement**
-- **Committee Management System**
-</t>
-  </si>
-  <si>
-    <t>### 2. Key Decisions Made</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- The Website Redesign wireframes are complete; development phase to begin imminently.
-- React with Next.js confirmed as the preferred tech stack for the Website Redesign.
-- Implementation of breadcrumb navigation system agreed for improved website navigation.
-- Mobile usability for the Website Redesign requires further adjustments; a comprehensive accessibility audit will be conducted.
-- Discord Bot meeting scheduling functionality nearly complete; notification system well-received though settings need clarity enhancements.
-- Advanced search filters to be added to the Discord Bot’s project tracking feature.
-- Bug fixes prioritized for Discord Bot reminders and Committee Management System duplicate user records.
-- Database query optimization and caching strategies progressing for the Committee Management System.
-- User permissions review underway to ensure proper access controls.
-- A shared UI component library to be established to maintain consistent design patterns across projects.
-- User survey will be conducted to gather feedback on Website Redesign color scheme and overall usability.
-</t>
-  </si>
-  <si>
-    <t>### 3. Action Items / Next Steps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**AI@DSCubed Website Redesign**  
-- Arnav: Finalize tech stack and coordinate CMS integration; implement breadcrumb navigation; coordinate with DevOps on CDN integration; collaborate with Fairy to contact UX team for error handling improvements.  
-- Chi: Conduct accessibility audit focusing on mobile responsiveness; liaise with Karen and design team on responsive breakpoints.  
-- Fairy: Contact UX team for best practices on user feedback and error handling.  
-- Karen: Confirm responsive design breakpoints and finalize color scheme survey distribution.
-**Discord Bot Enhancement**  
-- Andy L: Complete bug fixes on meeting reminders; draft content for project milestones timeline; test automated workflows; write data validation scripts; ensure performance optimization roadmap.  
-- Andy S: Finish calendar integration; enhance notification settings with added tooltips; initiate timeline feature development.  
-- Aaron: Refine notification settings; review system integration points; prepare rollback plan.  
-- Chi: Suggest adding export functionality to backlog; monitor user feedback on UI/UX.
-**Committee Management System**  
-- Andy S: Optimize database queries; set up monitoring and alerts for system performance; automate user onboarding; review user roles/permissions.  
-- Arnav: Implement unique constraints to prevent duplicate records; finalize database schema; coordinate with DevOps for caching/CDN; explore Slack integration for performance alerts.  
-- Andy L: Write scripts for data integrity validation; test automated workflows.
-</t>
-  </si>
-  <si>
-    <t>### 4. Relevant Projects Connected to Discussions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- **AI@DSCubed Website Redesign:** UX improvements, tech stack finalization, navigation restructuring, CMS integration, responsive/mobile design.
-- **Discord Bot Enhancement:** Meeting scheduling, notifications, accessibility, new timeline feature, project tracking improvements.
-- **Committee Management System:** Database performance, user permissions, onboarding automation, data integrity, monitoring.
-</t>
-  </si>
-  <si>
-    <t>### 5. Participant Contributions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- **Aaron:** Project oversight, bug identification, rollback planning, action item summarization.  
-- **Andy S:** Website development lead, analytics dashboard optimization, Discord Bot calendar and notification improvements, Committee Management System query optimization.  
-- **Andy L:** Discord Bot feature development, Committee Management System testing and automation, content drafting.  
-- **Arnav:** Technology stack research and implementation lead, database schema and constraints, DevOps coordination, UX improvements coordination.  
-- **Chi:** Accessibility and usability auditing, UI feedback, suggesting monitoring enhancements and features backlog.  
-- **Fairy:** UX liaison for Website Redesign error handling and feedback.  
-- **Karen:** Design team coordination on responsive breakpoints and color scheme.
-</t>
-  </si>
-  <si>
-    <t>### 6. Deadlines and Milestones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Development phase for Website Redesign to commence soon following wireframe approval.
-- Accessibility audit and mobile testing scheduled ahead of mobile version release.
-- Follow-up meetings for each project scheduled next week to review progress and next steps.
-- User survey on Website redesign color scheme and usability to be distributed promptly.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Summary Conclusion:**  </t>
-  </si>
-  <si>
-    <t>The meeting efficiently covered substantial progress and upcoming priorities across three key projects—AI@DSCubed Website Redesign, Discord Bot Enhancement, and Committee Management System. Clear action items were assigned with an emphasis on user experience, technical robustness, and design consistency. The team emphasized cross-project collaboration, particularly the establishment of a shared component library to unify design standards. Upcoming deadlines focus on transitioning designs into development, accessibility validation, and enhanced system monitoring. Follow-up meetings are set to ensure accountability and sustained momentum.</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -156,43 +49,94 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -480,87 +424,257 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="47.77734375" customWidth="1"/>
-    <col min="2" max="2" width="255.77734375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>topic_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>topic_name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>topic_description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>meeting_id</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ingestion_timestep</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Meeting Info</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**Meeting Summary**
+**Date:** [Not specified]  
+**Participants:** Aaron, Andy L, Andy S, Arnav, Chi, Fairy, Karen
+</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>45875</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Deadlines and Milestones</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- Development phase for Website Redesign to commence soon following wireframe approval.
+- Accessibility audit and mobile testing scheduled ahead of mobile version release.
+- Follow-up meetings for each project scheduled next week to review progress and next steps.
+- User survey on Website redesign color scheme and usability to be distributed promptly.
+</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>45875</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Main Topics Discussed</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- **AI@DSCubed Website Redesign**
+- **Discord Bot Enhancement**
+- **Committee Management System**
+</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>45875</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Key Decisions Made</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- The Website Redesign wireframes are complete; development phase to begin imminently.
+- React with Next.js confirmed as the preferred tech stack for the Website Redesign.
+- Implementation of breadcrumb navigation system agreed for improved website navigation.
+- Mobile usability for the Website Redesign requires further adjustments; a comprehensive accessibility audit will be conducted.
+- Discord Bot meeting scheduling functionality nearly complete; notification system well-received though settings need clarity enhancements.
+- Advanced search filters to be added to the Discord Bot’s project tracking feature.
+- Bug fixes prioritized for Discord Bot reminders and Committee Management System duplicate user records.
+- Database query optimization and caching strategies progressing for the Committee Management System.
+- User permissions review underway to ensure proper access controls.
+- A shared UI component library to be established to maintain consistent design patterns across projects.
+- User survey will be conducted to gather feedback on Website Redesign color scheme and overall usability.
+</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>45875</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Action Items / Next Steps</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">**AI@DSCubed Website Redesign**  
+- Arnav: Finalize tech stack and coordinate CMS integration; implement breadcrumb navigation; coordinate with DevOps on CDN integration; collaborate with Fairy to contact UX team for error handling improvements.  
+- Chi: Conduct accessibility audit focusing on mobile responsiveness; liaise with Karen and design team on responsive breakpoints.  
+- Fairy: Contact UX team for best practices on user feedback and error handling.  
+- Karen: Confirm responsive design breakpoints and finalize color scheme survey distribution.
+**Discord Bot Enhancement**  
+- Andy L: Complete bug fixes on meeting reminders; draft content for project milestones timeline; test automated workflows; write data validation scripts; ensure performance optimization roadmap.  
+- Andy S: Finish calendar integration; enhance notification settings with added tooltips; initiate timeline feature development.  
+- Aaron: Refine notification settings; review system integration points; prepare rollback plan.  
+- Chi: Suggest adding export functionality to backlog; monitor user feedback on UI/UX.
+**Committee Management System**  
+- Andy S: Optimize database queries; set up monitoring and alerts for system performance; automate user onboarding; review user roles/permissions.  
+- Arnav: Implement unique constraints to prevent duplicate records; finalize database schema; coordinate with DevOps for caching/CDN; explore Slack integration for performance alerts.  
+- Andy L: Write scripts for data integrity validation; test automated workflows.
+</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>45875</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Relevant Projects Connected to Discussions</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- **AI@DSCubed Website Redesign:** UX improvements, tech stack finalization, navigation restructuring, CMS integration, responsive/mobile design.
+- **Discord Bot Enhancement:** Meeting scheduling, notifications, accessibility, new timeline feature, project tracking improvements.
+- **Committee Management System:** Database performance, user permissions, onboarding automation, data integrity, monitoring.
+</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>45875</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Participant Contributions</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">- **Aaron:** Project oversight, bug identification, rollback planning, action item summarization.  
+- **Andy S:** Website development lead, analytics dashboard optimization, Discord Bot calendar and notification improvements, Committee Management System query optimization.  
+- **Andy L:** Discord Bot feature development, Committee Management System testing and automation, content drafting.  
+- **Arnav:** Technology stack research and implementation lead, database schema and constraints, DevOps coordination, UX improvements coordination.  
+- **Chi:** Accessibility and usability auditing, UI feedback, suggesting monitoring enhancements and features backlog.  
+- **Fairy:** UX liaison for Website Redesign error handling and feedback.  
+- **Karen:** Design team coordination on responsive breakpoints and color scheme.
+</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>45875</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
-        <v>17</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Summary Conclusion:  </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>The meeting efficiently covered substantial progress and upcoming priorities across three key projects—AI@DSCubed Website Redesign, Discord Bot Enhancement, and Committee Management System. Clear action items were assigned with an emphasis on user experience, technical robustness, and design consistency. The team emphasized cross-project collaboration, particularly the establishment of a shared component library to unify design standards. Upcoming deadlines focus on transitioning designs into development, accessibility validation, and enhanced system monitoring. Follow-up meetings are set to ensure accountability and sustained momentum.</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>45875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edited output_processor to describe function
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,20 +445,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>topic_name</t>
+          <t>topic_description</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>topic_description</t>
+          <t>meeting_id</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>meeting_id</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>ingestion_timestep</t>
         </is>
@@ -469,11 +464,6 @@
         <v>9</v>
       </c>
       <c r="B2" t="inlineStr">
-        <is>
-          <t>Meeting Info</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
         <is>
           <t xml:space="preserve">**Meeting Summary**
 **Date:** [Not specified]  
@@ -481,10 +471,10 @@
 </t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="n">
+      <c r="C2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="n">
         <v>45875</v>
       </c>
     </row>
@@ -493,11 +483,6 @@
         <v>15</v>
       </c>
       <c r="B3" t="inlineStr">
-        <is>
-          <t>Deadlines and Milestones</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve">- Development phase for Website Redesign to commence soon following wireframe approval.
 - Accessibility audit and mobile testing scheduled ahead of mobile version release.
@@ -506,10 +491,10 @@
 </t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="n">
+      <c r="C3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>45875</v>
       </c>
     </row>
@@ -518,11 +503,6 @@
         <v>10</v>
       </c>
       <c r="B4" t="inlineStr">
-        <is>
-          <t>Main Topics Discussed</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve">- **AI@DSCubed Website Redesign**
 - **Discord Bot Enhancement**
@@ -530,10 +510,10 @@
 </t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="n">
+      <c r="C4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>45875</v>
       </c>
     </row>
@@ -542,11 +522,6 @@
         <v>11</v>
       </c>
       <c r="B5" t="inlineStr">
-        <is>
-          <t>Key Decisions Made</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
         <is>
           <t xml:space="preserve">- The Website Redesign wireframes are complete; development phase to begin imminently.
 - React with Next.js confirmed as the preferred tech stack for the Website Redesign.
@@ -562,10 +537,10 @@
 </t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="n">
+      <c r="C5" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="n">
         <v>45875</v>
       </c>
     </row>
@@ -574,11 +549,6 @@
         <v>12</v>
       </c>
       <c r="B6" t="inlineStr">
-        <is>
-          <t>Action Items / Next Steps</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
         <is>
           <t xml:space="preserve">**AI@DSCubed Website Redesign**  
 - Arnav: Finalize tech stack and coordinate CMS integration; implement breadcrumb navigation; coordinate with DevOps on CDN integration; collaborate with Fairy to contact UX team for error handling improvements.  
@@ -597,10 +567,10 @@
 </t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="n">
+      <c r="C6" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="n">
         <v>45875</v>
       </c>
     </row>
@@ -609,11 +579,6 @@
         <v>13</v>
       </c>
       <c r="B7" t="inlineStr">
-        <is>
-          <t>Relevant Projects Connected to Discussions</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
         <is>
           <t xml:space="preserve">- **AI@DSCubed Website Redesign:** UX improvements, tech stack finalization, navigation restructuring, CMS integration, responsive/mobile design.
 - **Discord Bot Enhancement:** Meeting scheduling, notifications, accessibility, new timeline feature, project tracking improvements.
@@ -621,10 +586,10 @@
 </t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>10</v>
-      </c>
-      <c r="E7" s="2" t="n">
+      <c r="C7" t="n">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="n">
         <v>45875</v>
       </c>
     </row>
@@ -633,11 +598,6 @@
         <v>14</v>
       </c>
       <c r="B8" t="inlineStr">
-        <is>
-          <t>Participant Contributions</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
         <is>
           <t xml:space="preserve">- **Aaron:** Project oversight, bug identification, rollback planning, action item summarization.  
 - **Andy S:** Website development lead, analytics dashboard optimization, Discord Bot calendar and notification improvements, Committee Management System query optimization.  
@@ -649,10 +609,10 @@
 </t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2" t="n">
+      <c r="C8" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="n">
         <v>45875</v>
       </c>
     </row>
@@ -662,18 +622,13 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Summary Conclusion:  </t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
           <t>The meeting efficiently covered substantial progress and upcoming priorities across three key projects—AI@DSCubed Website Redesign, Discord Bot Enhancement, and Committee Management System. Clear action items were assigned with an emphasis on user experience, technical robustness, and design consistency. The team emphasized cross-project collaboration, particularly the establishment of a shared component library to unify design standards. Upcoming deadlines focus on transitioning designs into development, accessibility validation, and enhanced system monitoring. Follow-up meetings are set to ensure accountability and sustained momentum.</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>10</v>
-      </c>
-      <c r="E9" s="2" t="n">
+      <c r="C9" t="n">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="n">
         <v>45875</v>
       </c>
     </row>

</xml_diff>